<commit_message>
Update standup meeting for sprint 3
Create and update the stand file for this sprint and the upcoming week objectives.
</commit_message>
<xml_diff>
--- a/Project_Files/GDP-02-Sprint03/Stand-up Meeting Sec03Team05 Sprint03.xlsx
+++ b/Project_Files/GDP-02-Sprint03/Stand-up Meeting Sec03Team05 Sprint03.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/FreebiesforNewbies/Project_Files/GDP-02-Sprint03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78F29BC-412B-42E3-99A2-8CD035611D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{E78F29BC-412B-42E3-99A2-8CD035611D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A6647D1-8F19-499B-B99F-5FC3D3F401EF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Daily Stand-up Meeting Report</t>
   </si>
@@ -146,6 +146,24 @@
     <t>1. What did I accomplish?       
 2.What will I do today?
 3.What obstacles are impeding my progress?</t>
+  </si>
+  <si>
+    <t>Done changes in layout adding relative layout for some attributes in event delete request and event detail activity which are overlapping.</t>
+  </si>
+  <si>
+    <t>Integrating UI with backend code</t>
+  </si>
+  <si>
+    <t>Integrated UI with backend</t>
+  </si>
+  <si>
+    <t>Creating demo layouts for Admin</t>
+  </si>
+  <si>
+    <t>Created demo layouts for admin</t>
+  </si>
+  <si>
+    <t>Creating UI for admin activities</t>
   </si>
 </sst>
 </file>
@@ -750,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1231,9 +1249,15 @@
       <c r="A17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1259,9 +1283,15 @@
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1">
       <c r="A18" s="10"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1287,9 +1317,15 @@
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1">
       <c r="A19" s="11"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>

</xml_diff>

<commit_message>
Added week03 sprint meeting templet
</commit_message>
<xml_diff>
--- a/Project_Files/GDP-02-Sprint03/Stand-up Meeting Sec03Team05 Sprint03.xlsx
+++ b/Project_Files/GDP-02-Sprint03/Stand-up Meeting Sec03Team05 Sprint03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/FreebiesforNewbies/Project_Files/GDP-02-Sprint03/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\GDP-02-Sprint03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{E78F29BC-412B-42E3-99A2-8CD035611D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A6647D1-8F19-499B-B99F-5FC3D3F401EF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B60B817-075F-4917-BD7B-855354BEF354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="420" windowWidth="19180" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Daily Stand-up Meeting Report</t>
   </si>
@@ -165,12 +165,30 @@
   <si>
     <t>Creating UI for admin activities</t>
   </si>
+  <si>
+    <t>We have completed backend code for eventupdaterequest query and created tables in database</t>
+  </si>
+  <si>
+    <t>I have worked on backend code for eventupdaterequestquery</t>
+  </si>
+  <si>
+    <t>Working on backend for databse</t>
+  </si>
+  <si>
+    <t>I will do changes on backend code for eventupdaterequest query</t>
+  </si>
+  <si>
+    <t>I will write backend code for eventdeleterequest query</t>
+  </si>
+  <si>
+    <t>I will do few changes on queries regarding event delete table.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,8 +238,19 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF252525"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,8 +275,20 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -499,11 +540,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -551,6 +652,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,7 +885,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1131,7 +1247,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="13.5" customHeight="1">
+    <row r="13" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A13" s="11"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1159,13 +1275,19 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="13.5" customHeight="1">
+    <row r="14" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="B14" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>28</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1189,11 +1311,17 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="13.5" customHeight="1">
+    <row r="15" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A15" s="10"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
+      <c r="B15" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>31</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1217,11 +1345,17 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="13.5" customHeight="1">
+    <row r="16" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>8</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -28855,6 +28989,6 @@
     <mergeCell ref="A14:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>